<commit_message>
start of project 3
ADL
</commit_message>
<xml_diff>
--- a/Project 4/results.xlsx
+++ b/Project 4/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josia\Documents\UNI Stuff\CS\24 25\Algorithms and Data Structures\CourseWork\ADS\Project 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CCAAC26-07B1-406F-93DF-B5EFB93E82CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468391C2-8610-4C33-99A0-D6B62750533E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{643723C8-895F-43D3-9120-2CB0ABC84852}"/>
   </bookViews>
@@ -19,6 +19,12 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'Results (2)'!$B$2:$B$101</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">'Results (2)'!$B$2:$B$101</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Results (2)'!$H$14:$H$14</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Results (2)'!#REF!</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Results (2)'!$H$101</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Results (2)'!$H$2:$H$100</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Results (2)'!$C$2:$C$101</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Results (2)'!$C$2:$C$101</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Results (2)'!$A$1:$E$101</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -50,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="208">
   <si>
     <t>9, 4, 1, 2, 4, 8, 3, 2, 3, 1, 9, 4, 10, 10, 14, 12, 11, 2, 7, 1, 11, 7, 9, 9, 1, 14, 5, 5, 3, 5</t>
   </si>
@@ -665,6 +671,15 @@
   </si>
   <si>
     <t xml:space="preserve">bins </t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>fitness</t>
   </si>
 </sst>
 </file>
@@ -700,9 +715,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1282,7 +1296,700 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Results (2)'!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77630769230769248</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.84099999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.91745454545454563</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Results (2)'!$H$2:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D307-40F4-B0FF-D50FC4FA615A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="473856559"/>
+        <c:axId val="473858959"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="473856559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="473858959"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="473858959"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="473856559"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Results (2)'!$G$2:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77630769230769248</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.84099999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.91745454545454563</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Results (2)'!$H$2:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-479D-4099-93BF-7DA7E69DEE65}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.6</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{13630349-76BD-425F-AC2A-6F61FC2D0959}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1838,6 +2545,1536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1874,6 +4111,156 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>13990543</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>124386</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>240925</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>10086</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D303B6FE-D519-85E3-101E-C1A15C285348}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5602</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>146797</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>252131</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>32497</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{875777F2-6C95-6466-C650-1910A1ADC8AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1451160</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>169208</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>10298205</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>168088</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="11" name="Chart 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9DAF841-4A21-EAF3-A21A-A1163E60EC74}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9463366" y="19790708"/>
+              <a:ext cx="8847045" cy="3427880"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2224,10 +4611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E4E6F0D-E78E-44E3-9BDA-F183B041162F}">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E125" sqref="E125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2237,9 +4624,10 @@
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="209.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>200</v>
       </c>
@@ -2255,9 +4643,15 @@
       <c r="E1" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="G1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -2269,12 +4663,22 @@
       <c r="D2">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="G2">
+        <v>-1</v>
+      </c>
+      <c r="H2">
+        <f>COUNTIFS(Results[Fitness],G2)</f>
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -2286,12 +4690,19 @@
       <c r="D3">
         <v>12</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="G3">
+        <v>0.77630769230769248</v>
+      </c>
+      <c r="H3">
+        <f>COUNTIFS(Results[Fitness],G3)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
@@ -2303,12 +4714,19 @@
       <c r="D4">
         <v>11</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="G4">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="H4">
+        <f>COUNTIFS(Results[Fitness],G4)</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5">
@@ -2320,12 +4738,19 @@
       <c r="D5">
         <v>12</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="G5">
+        <v>0.91745454545454563</v>
+      </c>
+      <c r="H5">
+        <f>COUNTIFS(Results[Fitness],G5)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6">
@@ -2337,12 +4762,12 @@
       <c r="D6">
         <v>12</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7">
@@ -2354,12 +4779,12 @@
       <c r="D7">
         <v>12</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8">
@@ -2371,12 +4796,12 @@
       <c r="D8">
         <v>12</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9">
@@ -2388,12 +4813,12 @@
       <c r="D9">
         <v>12</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10">
@@ -2405,12 +4830,12 @@
       <c r="D10">
         <v>10</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11">
@@ -2422,12 +4847,12 @@
       <c r="D11">
         <v>12</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12">
@@ -2439,12 +4864,12 @@
       <c r="D12">
         <v>12</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13">
@@ -2456,12 +4881,12 @@
       <c r="D13">
         <v>11</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14">
@@ -2473,12 +4898,12 @@
       <c r="D14">
         <v>9</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>26</v>
       </c>
       <c r="B15">
@@ -2490,12 +4915,12 @@
       <c r="D15">
         <v>12</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>28</v>
       </c>
       <c r="B16">
@@ -2507,12 +4932,12 @@
       <c r="D16">
         <v>11</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>30</v>
       </c>
       <c r="B17">
@@ -2524,12 +4949,12 @@
       <c r="D17">
         <v>12</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>32</v>
       </c>
       <c r="B18">
@@ -2541,12 +4966,12 @@
       <c r="D18">
         <v>12</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>34</v>
       </c>
       <c r="B19">
@@ -2558,12 +4983,12 @@
       <c r="D19">
         <v>12</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>36</v>
       </c>
       <c r="B20">
@@ -2575,12 +5000,12 @@
       <c r="D20">
         <v>12</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>38</v>
       </c>
       <c r="B21">
@@ -2592,12 +5017,12 @@
       <c r="D21">
         <v>12</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>40</v>
       </c>
       <c r="B22">
@@ -2609,12 +5034,12 @@
       <c r="D22">
         <v>11</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>42</v>
       </c>
       <c r="B23">
@@ -2626,12 +5051,12 @@
       <c r="D23">
         <v>12</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>44</v>
       </c>
       <c r="B24">
@@ -2643,12 +5068,12 @@
       <c r="D24">
         <v>12</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>46</v>
       </c>
       <c r="B25">
@@ -2660,12 +5085,12 @@
       <c r="D25">
         <v>11</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>48</v>
       </c>
       <c r="B26">
@@ -2677,12 +5102,12 @@
       <c r="D26">
         <v>10</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>50</v>
       </c>
       <c r="B27">
@@ -2694,12 +5119,12 @@
       <c r="D27">
         <v>12</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>52</v>
       </c>
       <c r="B28">
@@ -2711,12 +5136,12 @@
       <c r="D28">
         <v>12</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>54</v>
       </c>
       <c r="B29">
@@ -2728,12 +5153,12 @@
       <c r="D29">
         <v>12</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>56</v>
       </c>
       <c r="B30">
@@ -2745,12 +5170,12 @@
       <c r="D30">
         <v>9</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>58</v>
       </c>
       <c r="B31">
@@ -2762,12 +5187,12 @@
       <c r="D31">
         <v>9</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>60</v>
       </c>
       <c r="B32">
@@ -2779,12 +5204,12 @@
       <c r="D32">
         <v>12</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>62</v>
       </c>
       <c r="B33">
@@ -2796,12 +5221,12 @@
       <c r="D33">
         <v>12</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>64</v>
       </c>
       <c r="B34">
@@ -2813,12 +5238,12 @@
       <c r="D34">
         <v>9</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>66</v>
       </c>
       <c r="B35">
@@ -2830,12 +5255,12 @@
       <c r="D35">
         <v>12</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>68</v>
       </c>
       <c r="B36">
@@ -2847,12 +5272,12 @@
       <c r="D36">
         <v>12</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>70</v>
       </c>
       <c r="B37">
@@ -2864,12 +5289,12 @@
       <c r="D37">
         <v>11</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>72</v>
       </c>
       <c r="B38">
@@ -2881,12 +5306,12 @@
       <c r="D38">
         <v>12</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>74</v>
       </c>
       <c r="B39">
@@ -2898,12 +5323,12 @@
       <c r="D39">
         <v>9</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>76</v>
       </c>
       <c r="B40">
@@ -2915,12 +5340,12 @@
       <c r="D40">
         <v>12</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>78</v>
       </c>
       <c r="B41">
@@ -2932,12 +5357,12 @@
       <c r="D41">
         <v>12</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="A42" t="s">
         <v>80</v>
       </c>
       <c r="B42">
@@ -2949,12 +5374,12 @@
       <c r="D42">
         <v>12</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>82</v>
       </c>
       <c r="B43">
@@ -2966,12 +5391,12 @@
       <c r="D43">
         <v>12</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="A44" t="s">
         <v>84</v>
       </c>
       <c r="B44">
@@ -2983,12 +5408,12 @@
       <c r="D44">
         <v>12</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="A45" t="s">
         <v>86</v>
       </c>
       <c r="B45">
@@ -3000,12 +5425,12 @@
       <c r="D45">
         <v>12</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>88</v>
       </c>
       <c r="B46">
@@ -3017,12 +5442,12 @@
       <c r="D46">
         <v>12</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>90</v>
       </c>
       <c r="B47">
@@ -3034,12 +5459,12 @@
       <c r="D47">
         <v>12</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>92</v>
       </c>
       <c r="B48">
@@ -3051,12 +5476,12 @@
       <c r="D48">
         <v>12</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="A49" t="s">
         <v>94</v>
       </c>
       <c r="B49">
@@ -3068,12 +5493,12 @@
       <c r="D49">
         <v>12</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="A50" t="s">
         <v>96</v>
       </c>
       <c r="B50">
@@ -3085,12 +5510,12 @@
       <c r="D50">
         <v>12</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="A51" t="s">
         <v>98</v>
       </c>
       <c r="B51">
@@ -3102,12 +5527,12 @@
       <c r="D51">
         <v>12</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="A52" t="s">
         <v>100</v>
       </c>
       <c r="B52">
@@ -3119,12 +5544,12 @@
       <c r="D52">
         <v>12</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E52" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="A53" t="s">
         <v>102</v>
       </c>
       <c r="B53">
@@ -3136,12 +5561,12 @@
       <c r="D53">
         <v>12</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E53" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="A54" t="s">
         <v>104</v>
       </c>
       <c r="B54">
@@ -3153,12 +5578,12 @@
       <c r="D54">
         <v>9</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E54" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="A55" t="s">
         <v>106</v>
       </c>
       <c r="B55">
@@ -3170,12 +5595,12 @@
       <c r="D55">
         <v>11</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E55" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="A56" t="s">
         <v>108</v>
       </c>
       <c r="B56">
@@ -3187,12 +5612,12 @@
       <c r="D56">
         <v>10</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E56" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="A57" t="s">
         <v>110</v>
       </c>
       <c r="B57">
@@ -3204,12 +5629,12 @@
       <c r="D57">
         <v>12</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E57" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="A58" t="s">
         <v>112</v>
       </c>
       <c r="B58">
@@ -3221,12 +5646,12 @@
       <c r="D58">
         <v>12</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E58" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+      <c r="A59" t="s">
         <v>114</v>
       </c>
       <c r="B59">
@@ -3238,12 +5663,12 @@
       <c r="D59">
         <v>12</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E59" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="A60" t="s">
         <v>116</v>
       </c>
       <c r="B60">
@@ -3255,12 +5680,12 @@
       <c r="D60">
         <v>12</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E60" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="A61" t="s">
         <v>118</v>
       </c>
       <c r="B61">
@@ -3272,12 +5697,12 @@
       <c r="D61">
         <v>12</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E61" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="A62" t="s">
         <v>120</v>
       </c>
       <c r="B62">
@@ -3289,12 +5714,12 @@
       <c r="D62">
         <v>10</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E62" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="A63" t="s">
         <v>122</v>
       </c>
       <c r="B63">
@@ -3306,12 +5731,12 @@
       <c r="D63">
         <v>12</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="E63" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+      <c r="A64" t="s">
         <v>124</v>
       </c>
       <c r="B64">
@@ -3323,12 +5748,12 @@
       <c r="D64">
         <v>12</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="E64" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+      <c r="A65" t="s">
         <v>126</v>
       </c>
       <c r="B65">
@@ -3340,12 +5765,12 @@
       <c r="D65">
         <v>11</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="E65" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="A66" t="s">
         <v>128</v>
       </c>
       <c r="B66">
@@ -3357,12 +5782,12 @@
       <c r="D66">
         <v>12</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E66" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+      <c r="A67" t="s">
         <v>130</v>
       </c>
       <c r="B67">
@@ -3374,12 +5799,12 @@
       <c r="D67">
         <v>13</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="E67" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+      <c r="A68" t="s">
         <v>132</v>
       </c>
       <c r="B68">
@@ -3391,12 +5816,12 @@
       <c r="D68">
         <v>12</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="E68" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="A69" t="s">
         <v>134</v>
       </c>
       <c r="B69">
@@ -3408,12 +5833,12 @@
       <c r="D69">
         <v>11</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="E69" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+      <c r="A70" t="s">
         <v>136</v>
       </c>
       <c r="B70">
@@ -3425,12 +5850,12 @@
       <c r="D70">
         <v>12</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E70" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+      <c r="A71" t="s">
         <v>138</v>
       </c>
       <c r="B71">
@@ -3442,12 +5867,12 @@
       <c r="D71">
         <v>12</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="E71" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+      <c r="A72" t="s">
         <v>140</v>
       </c>
       <c r="B72">
@@ -3459,12 +5884,12 @@
       <c r="D72">
         <v>12</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="E72" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+      <c r="A73" t="s">
         <v>142</v>
       </c>
       <c r="B73">
@@ -3476,12 +5901,12 @@
       <c r="D73">
         <v>12</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="E73" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+      <c r="A74" t="s">
         <v>144</v>
       </c>
       <c r="B74">
@@ -3493,12 +5918,12 @@
       <c r="D74">
         <v>10</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="E74" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+      <c r="A75" t="s">
         <v>146</v>
       </c>
       <c r="B75">
@@ -3510,16 +5935,16 @@
       <c r="D75">
         <v>12</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="E75" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+      <c r="A76" t="s">
         <v>148</v>
       </c>
       <c r="B76">
-        <v>0.84100000000000019</v>
+        <v>0.84099999999999997</v>
       </c>
       <c r="C76">
         <v>317538</v>
@@ -3527,12 +5952,12 @@
       <c r="D76">
         <v>12</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="E76" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+      <c r="A77" t="s">
         <v>150</v>
       </c>
       <c r="B77">
@@ -3544,12 +5969,12 @@
       <c r="D77">
         <v>12</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="E77" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+      <c r="A78" t="s">
         <v>152</v>
       </c>
       <c r="B78">
@@ -3561,12 +5986,12 @@
       <c r="D78">
         <v>12</v>
       </c>
-      <c r="E78" s="1" t="s">
+      <c r="E78" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+      <c r="A79" t="s">
         <v>154</v>
       </c>
       <c r="B79">
@@ -3578,12 +6003,12 @@
       <c r="D79">
         <v>11</v>
       </c>
-      <c r="E79" s="1" t="s">
+      <c r="E79" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+      <c r="A80" t="s">
         <v>156</v>
       </c>
       <c r="B80">
@@ -3595,12 +6020,12 @@
       <c r="D80">
         <v>11</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="E80" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+      <c r="A81" t="s">
         <v>158</v>
       </c>
       <c r="B81">
@@ -3612,12 +6037,12 @@
       <c r="D81">
         <v>12</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="E81" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+      <c r="A82" t="s">
         <v>160</v>
       </c>
       <c r="B82">
@@ -3629,12 +6054,12 @@
       <c r="D82">
         <v>11</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="E82" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+      <c r="A83" t="s">
         <v>162</v>
       </c>
       <c r="B83">
@@ -3646,12 +6071,12 @@
       <c r="D83">
         <v>13</v>
       </c>
-      <c r="E83" s="1" t="s">
+      <c r="E83" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+      <c r="A84" t="s">
         <v>164</v>
       </c>
       <c r="B84">
@@ -3663,12 +6088,12 @@
       <c r="D84">
         <v>12</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="E84" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+      <c r="A85" t="s">
         <v>166</v>
       </c>
       <c r="B85">
@@ -3680,12 +6105,12 @@
       <c r="D85">
         <v>12</v>
       </c>
-      <c r="E85" s="1" t="s">
+      <c r="E85" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+      <c r="A86" t="s">
         <v>168</v>
       </c>
       <c r="B86">
@@ -3697,12 +6122,12 @@
       <c r="D86">
         <v>10</v>
       </c>
-      <c r="E86" s="1" t="s">
+      <c r="E86" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+      <c r="A87" t="s">
         <v>170</v>
       </c>
       <c r="B87">
@@ -3714,12 +6139,12 @@
       <c r="D87">
         <v>12</v>
       </c>
-      <c r="E87" s="1" t="s">
+      <c r="E87" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+      <c r="A88" t="s">
         <v>172</v>
       </c>
       <c r="B88">
@@ -3731,12 +6156,12 @@
       <c r="D88">
         <v>11</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="E88" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+      <c r="A89" t="s">
         <v>174</v>
       </c>
       <c r="B89">
@@ -3748,12 +6173,12 @@
       <c r="D89">
         <v>11</v>
       </c>
-      <c r="E89" s="1" t="s">
+      <c r="E89" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+      <c r="A90" t="s">
         <v>176</v>
       </c>
       <c r="B90">
@@ -3765,12 +6190,12 @@
       <c r="D90">
         <v>12</v>
       </c>
-      <c r="E90" s="1" t="s">
+      <c r="E90" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+      <c r="A91" t="s">
         <v>178</v>
       </c>
       <c r="B91">
@@ -3782,12 +6207,12 @@
       <c r="D91">
         <v>13</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="E91" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+      <c r="A92" t="s">
         <v>180</v>
       </c>
       <c r="B92">
@@ -3799,12 +6224,12 @@
       <c r="D92">
         <v>12</v>
       </c>
-      <c r="E92" s="1" t="s">
+      <c r="E92" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+      <c r="A93" t="s">
         <v>182</v>
       </c>
       <c r="B93">
@@ -3816,12 +6241,12 @@
       <c r="D93">
         <v>10</v>
       </c>
-      <c r="E93" s="1" t="s">
+      <c r="E93" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+      <c r="A94" t="s">
         <v>184</v>
       </c>
       <c r="B94">
@@ -3833,12 +6258,12 @@
       <c r="D94">
         <v>10</v>
       </c>
-      <c r="E94" s="1" t="s">
+      <c r="E94" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+      <c r="A95" t="s">
         <v>186</v>
       </c>
       <c r="B95">
@@ -3850,12 +6275,12 @@
       <c r="D95">
         <v>12</v>
       </c>
-      <c r="E95" s="1" t="s">
+      <c r="E95" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+      <c r="A96" t="s">
         <v>188</v>
       </c>
       <c r="B96">
@@ -3867,12 +6292,12 @@
       <c r="D96">
         <v>9</v>
       </c>
-      <c r="E96" s="1" t="s">
+      <c r="E96" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+      <c r="A97" t="s">
         <v>190</v>
       </c>
       <c r="B97">
@@ -3884,12 +6309,12 @@
       <c r="D97">
         <v>12</v>
       </c>
-      <c r="E97" s="1" t="s">
+      <c r="E97" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+      <c r="A98" t="s">
         <v>192</v>
       </c>
       <c r="B98">
@@ -3901,12 +6326,12 @@
       <c r="D98">
         <v>12</v>
       </c>
-      <c r="E98" s="1" t="s">
+      <c r="E98" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+      <c r="A99" t="s">
         <v>194</v>
       </c>
       <c r="B99">
@@ -3918,12 +6343,12 @@
       <c r="D99">
         <v>12</v>
       </c>
-      <c r="E99" s="1" t="s">
+      <c r="E99" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+      <c r="A100" t="s">
         <v>196</v>
       </c>
       <c r="B100">
@@ -3935,12 +6360,12 @@
       <c r="D100">
         <v>10</v>
       </c>
-      <c r="E100" s="1" t="s">
+      <c r="E100" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+      <c r="A101" t="s">
         <v>198</v>
       </c>
       <c r="B101">
@@ -3952,11 +6377,14 @@
       <c r="D101">
         <v>10</v>
       </c>
-      <c r="E101" s="1" t="s">
+      <c r="E101" t="s">
         <v>199</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G2:H5">
+    <sortCondition ref="G2:G5"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
project 4 doc clean up + videos
</commit_message>
<xml_diff>
--- a/Project 4/results.xlsx
+++ b/Project 4/results.xlsx
@@ -8,19 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FiercePC\Documents\GitHub\ADS\Project 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C958656-21E9-432E-B7CA-D663358ACC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FB347C-7A82-4AB0-B891-F50588BE6F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{643723C8-895F-43D3-9120-2CB0ABC84852}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" xr2:uid="{643723C8-895F-43D3-9120-2CB0ABC84852}"/>
   </bookViews>
   <sheets>
-    <sheet name="Results (2)" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
-    <sheet name="Results" sheetId="1" r:id="rId4"/>
+    <sheet name="Results" sheetId="2" r:id="rId1"/>
+    <sheet name="fitness" sheetId="3" r:id="rId2"/>
+    <sheet name="numBins" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Results (2)'!$C$2:$C$101</definedName>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Results (2)'!$A$1:$E$101</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Results'!$C$2:$C$101</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Results'!$A$1:$E$101</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -689,7 +688,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -730,7 +729,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -802,561 +801,6 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.12631364829396324"/>
-          <c:y val="0.1861945902595509"/>
-          <c:w val="0.8396412948381452"/>
-          <c:h val="0.72989246135899677"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Results (2)'!$C$2:$C$101</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
-                <c:pt idx="0">
-                  <c:v>601959</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>544124</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>881338</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>416063</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1882405</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1235240</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>475026</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1169697</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2000176</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>537977</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>911330</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>744647</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2000573</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>557422</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>628479</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1074290</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1233361</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>911758</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>606162</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>689542</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>436610</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>833796</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>805172</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1663595</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2010608</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>631927</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1834867</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1201307</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2000189</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2000199</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1472236</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1781624</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2002558</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>578346</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>901068</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>664415</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1853725</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>2000082</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>627950</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>444871</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>393075</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>992138</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>615235</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>728787</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>892476</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>718759</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>466225</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>1743653</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>546079</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>436182</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>878450</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>715787</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>2002069</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>531411</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>2000120</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>1185705</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>663882</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>1158333</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>673895</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>572507</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>2000018</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>792540</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>913977</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>724412</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>922359</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>1787192</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>1113454</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>599930</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>1059482</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>1233892</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>769776</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>1228381</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>2000273</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>2170393</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>317538</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>1504768</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>792011</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>686306</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>996307</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>1076556</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>374362</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>1633294</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>1313388</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>862715</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>2000394</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>1689394</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>848272</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>672611</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>443536</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>611909</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>1447393</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>2004584</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>2000146</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>1941035</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>2006421</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>1116148</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>305332</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>1290925</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>2004281</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>2001794</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-ACD1-40A7-8F03-FBA3D857D03E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="1197086672"/>
-        <c:axId val="1197090032"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1197086672"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1197090032"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1197090032"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1197086672"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
@@ -1377,7 +821,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Results (2)'!$G$2:$G$5</c:f>
+              <c:f>'Results'!$G$2:$G$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1398,7 +842,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Results (2)'!$H$2:$H$5</c:f>
+              <c:f>'Results'!$H$2:$H$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1588,7 +1032,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1742,7 +1186,7 @@
           </c:dPt>
           <c:cat>
             <c:numRef>
-              <c:f>'Results (2)'!$G$2:$G$6</c:f>
+              <c:f>'Results'!$G$2:$G$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1763,7 +1207,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Results (2)'!$H$2:$H$6</c:f>
+              <c:f>'Results'!$H$2:$H$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1875,910 +1319,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Results (2)'!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>iterations</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Results (2)'!$B$2:$B$101</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
-                <c:pt idx="0">
-                  <c:v>0.84099999999999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.91745454545454563</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.91745454545454563</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.91745454545454563</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.8410000000000003</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.91745454545454563</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.8410000000000003</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.8410000000000003</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.91745454545454552</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.91745454545454563</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.8410000000000003</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.84100000000000008</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.8410000000000003</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0.91745454545454552</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>0.91745454545454552</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0.77630769230769248</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0.91745454545454552</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>0.84099999999999997</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.8410000000000003</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>0.91745454545454552</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0.91745454545454552</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>0.84100000000000008</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.91745454545454552</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0.77630769230769248</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.91745454545454552</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.91745454545454552</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.77630769230769248</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0.84100000000000019</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>-1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Results (2)'!$C$2:$C$101</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
-                <c:pt idx="0">
-                  <c:v>601959</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>544124</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>881338</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>416063</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1882405</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1235240</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>475026</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1169697</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2000176</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>537977</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>911330</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>744647</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2000573</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>557422</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>628479</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1074290</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1233361</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>911758</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>606162</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>689542</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>436610</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>833796</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>805172</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1663595</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2010608</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>631927</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1834867</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1201307</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2000189</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2000199</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1472236</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1781624</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2002558</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>578346</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>901068</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>664415</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1853725</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>2000082</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>627950</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>444871</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>393075</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>992138</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>615235</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>728787</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>892476</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>718759</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>466225</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>1743653</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>546079</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>436182</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>878450</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>715787</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>2002069</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>531411</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>2000120</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>1185705</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>663882</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>1158333</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>673895</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>572507</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>2000018</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>792540</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>913977</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>724412</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>922359</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>1787192</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>1113454</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>599930</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>1059482</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>1233892</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>769776</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>1228381</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>2000273</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>2170393</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>317538</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>1504768</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>792011</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>686306</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>996307</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>1076556</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>374362</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>1633294</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>1313388</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>862715</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>2000394</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>1689394</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>848272</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>672611</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>443536</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>611909</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>1447393</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>2004584</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>2000146</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>1941035</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>2006421</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>1116148</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>305332</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>1290925</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>2004281</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>2001794</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3DBA-4601-8928-ED0224BFEFDF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="116415856"/>
-        <c:axId val="116415376"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="116415856"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="116415376"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="116415376"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="116415856"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2833,7 +1374,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>fitness!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2866,7 +1407,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$101</c:f>
+              <c:f>fitness!$A$2:$A$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -3175,7 +1716,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$101</c:f>
+              <c:f>fitness!$B$2:$B$101</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="100"/>
@@ -3728,7 +2269,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3783,7 +2324,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$B$1</c:f>
+              <c:f>numBins!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3816,7 +2357,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$A$2:$A$101</c:f>
+              <c:f>numBins!$A$2:$A$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -4125,7 +2666,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$B$101</c:f>
+              <c:f>numBins!$B$2:$B$101</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="100"/>
@@ -4681,40 +3222,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
-<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
-  <cx:chartData>
-    <cx:data id="0">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.0</cx:f>
-      </cx:numDim>
-    </cx:data>
-  </cx:chartData>
-  <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
-    <cx:plotArea>
-      <cx:plotAreaRegion>
-        <cx:series layoutId="clusteredColumn" uniqueId="{13630349-76BD-425F-AC2A-6F61FC2D0959}">
-          <cx:dataId val="0"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-      </cx:plotAreaRegion>
-      <cx:axis id="0">
-        <cx:catScaling gapWidth="0"/>
-        <cx:tickLabels/>
-      </cx:axis>
-      <cx:axis id="1">
-        <cx:valScaling/>
-        <cx:majorGridlines/>
-        <cx:tickLabels/>
-      </cx:axis>
-    </cx:plotArea>
-  </cx:chart>
-</cx:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4875,128 +3382,8 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5104,11 +3491,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -5119,11 +3501,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -5155,9 +3532,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5512,7 +3886,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5569,7 +3943,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -5620,6 +3994,13 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -5630,12 +4011,19 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -5673,7 +4061,7 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -5716,22 +4104,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -5836,8 +4225,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5969,19 +4358,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -6015,7 +4405,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -6042,8 +4432,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6072,7 +4462,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -6123,13 +4513,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -6140,25 +4523,18 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -6193,7 +4569,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -6514,6 +4890,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -6534,7 +4921,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -6545,7 +4932,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -6561,516 +4948,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
             <a:lumMod val="25000"/>
             <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat">
-        <a:solidFill>
-          <a:srgbClr val="D9D9D9"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -7150,522 +5029,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -8073,560 +5436,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>3510243</xdr:colOff>
-      <xdr:row>107</xdr:row>
-      <xdr:rowOff>49586</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>62193</xdr:colOff>
-      <xdr:row>121</xdr:row>
-      <xdr:rowOff>125786</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95547384-1FE8-9F8B-0434-DDE168A88411}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -8657,7 +5468,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8693,121 +5504,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1451160</xdr:colOff>
-      <xdr:row>103</xdr:row>
-      <xdr:rowOff>169208</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>10298205</xdr:colOff>
-      <xdr:row>121</xdr:row>
-      <xdr:rowOff>168088</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="11" name="Chart 10">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9DAF841-4A21-EAF3-A21A-A1163E60EC74}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="9471210" y="19790708"/>
-              <a:ext cx="8847045" cy="3427880"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100"/>
-                <a:t>This chart isn't available in your version of Excel.
-Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>7681631</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>118782</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>156882</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>33617</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2095ED8E-9D3D-79FD-152C-855E0EE01C4A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9247,8 +5944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E4E6F0D-E78E-44E3-9BDA-F183B041162F}">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D101"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11032,7 +7729,7 @@
   <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J82" sqref="A1:XFD1048576"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11861,7 +8558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36FB3BAA-CDF5-474D-BD23-C1B282EEA2B0}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AC27" sqref="AC27"/>
     </sheetView>
   </sheetViews>
@@ -12682,23 +9379,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FD2C00B-F037-4804-A8AF-C623DD0C9B0C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="255.7109375" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>